<commit_message>
loop through eims mods per-cruise then assemble
</commit_message>
<xml_diff>
--- a/ncp-gop-transect-summer-2018/gop-transect-en617.xlsx
+++ b/ncp-gop-transect-summer-2018/gop-transect-en617.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>attributeName</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>character</t>
+  </si>
+  <si>
+    <t>iode_quality_flag</t>
+  </si>
+  <si>
+    <t>flag</t>
   </si>
 </sst>
 </file>
@@ -501,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -703,6 +709,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>